<commit_message>
Drafted analyses for gender effect, corrected one coding (which did not contain enough info but accidentally did get final coding)
</commit_message>
<xml_diff>
--- a/gender/gendercoded cleaned and discussed.xlsx
+++ b/gender/gendercoded cleaned and discussed.xlsx
@@ -298,7 +298,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="378">
   <si>
     <t>chjh</t>
   </si>
@@ -1813,8 +1813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L181"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2362,9 +2362,8 @@
       <c r="E15" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="L15" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v>no expectation</v>
+      <c r="L15" s="1" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="300" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Moved around a lot of files, had to recompute the gendercoded cleaned and discussed p-values because of something going wrong with scipen... drafted gender analyses
</commit_message>
<xml_diff>
--- a/gender/gendercoded cleaned and discussed.xlsx
+++ b/gender/gendercoded cleaned and discussed.xlsx
@@ -1530,7 +1530,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1813,8 +1813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D106" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1822,6 +1822,7 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="27.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="36.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="51.140625" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -1836,7 +1837,7 @@
       <c r="C1" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>377</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -1874,7 +1875,7 @@
       <c r="C2" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>4.5606043365487202E-2</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -1911,7 +1912,7 @@
       <c r="C3" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>2.8829046514401799E-2</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -1949,7 +1950,7 @@
         <v>374</v>
       </c>
       <c r="D4" s="9">
-        <v>60.212559622348699</v>
+        <v>6.0212559622348699E-13</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>285</v>
@@ -1986,7 +1987,7 @@
         <v>374</v>
       </c>
       <c r="D5" s="9">
-        <v>9392354759.2166691</v>
+        <v>9.3923547592166695E-5</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>239</v>
@@ -2022,7 +2023,7 @@
       <c r="C6" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>0.14692397586190001</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -2059,7 +2060,7 @@
       <c r="C7" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>8.7341610036581196E-3</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -2096,7 +2097,7 @@
       <c r="C8" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>0.39209154480973801</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -2133,7 +2134,7 @@
       <c r="C9" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>0.25421322360396398</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -2170,7 +2171,7 @@
       <c r="C10" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>1.24252580422006E-2</v>
       </c>
       <c r="E10" s="2" t="s">
@@ -2207,7 +2208,7 @@
       <c r="C11" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>1.1217494509396899E-2</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -2244,7 +2245,7 @@
       <c r="C12" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>5.4682168971339602E-2</v>
       </c>
       <c r="E12" s="2" t="s">
@@ -2283,7 +2284,7 @@
       <c r="C13" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>1.37581367440372E-4</v>
       </c>
       <c r="E13" s="2" t="s">
@@ -2319,7 +2320,7 @@
       <c r="C14" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>0.65478498578714295</v>
       </c>
       <c r="E14" s="2" t="s">
@@ -2357,7 +2358,7 @@
         <v>374</v>
       </c>
       <c r="D15" s="9">
-        <v>4394445221.49016</v>
+        <v>4.3944452214901598E-5</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>242</v>
@@ -2376,7 +2377,7 @@
       <c r="C16" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>7.5906227509229601E-3</v>
       </c>
       <c r="E16" s="2" t="s">
@@ -2413,7 +2414,7 @@
       <c r="C17" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>6.2114739723029999E-2</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -2449,7 +2450,7 @@
       <c r="C18" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>0.33133143283533101</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -2486,7 +2487,7 @@
       <c r="C19" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>0.28717123916026099</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -2524,7 +2525,7 @@
         <v>374</v>
       </c>
       <c r="D20" s="9">
-        <v>7621748336.3689604</v>
+        <v>7.6217483363689602E-5</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>289</v>
@@ -2561,7 +2562,7 @@
         <v>374</v>
       </c>
       <c r="D21" s="9">
-        <v>6.6876091427906995E-5</v>
+        <v>6.6876091427907002E-18</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>280</v>
@@ -2597,7 +2598,7 @@
       <c r="C22" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>0.99600832130982497</v>
       </c>
       <c r="E22" s="2" t="s">
@@ -2634,7 +2635,7 @@
       <c r="C23" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>0.37446861988792302</v>
       </c>
       <c r="E23" s="5" t="s">
@@ -2672,7 +2673,7 @@
         <v>374</v>
       </c>
       <c r="D24" s="9">
-        <v>3.3188417399295699E-4</v>
+        <v>3.3188417399295701E-18</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>327</v>
@@ -2708,7 +2709,7 @@
       <c r="C25" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>9.6898694236794605E-2</v>
       </c>
       <c r="E25" s="2" t="s">
@@ -2746,7 +2747,7 @@
         <v>374</v>
       </c>
       <c r="D26" s="9">
-        <v>3.25902219580641E-12</v>
+        <v>3.2590221958064098E-26</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>238</v>
@@ -2782,7 +2783,7 @@
       <c r="C27" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>0.545554389362644</v>
       </c>
       <c r="E27" s="2" t="s">
@@ -2819,7 +2820,7 @@
       <c r="C28" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>0.98271479448916699</v>
       </c>
       <c r="E28" s="2" t="s">
@@ -2856,7 +2857,7 @@
       <c r="C29" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>0.96079447849125799</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -2894,7 +2895,7 @@
         <v>374</v>
       </c>
       <c r="D30" s="9">
-        <v>91867189.883412406</v>
+        <v>9.1867189883412396E-7</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>324</v>
@@ -2930,7 +2931,7 @@
       <c r="C31" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>4.6483591207729297E-2</v>
       </c>
       <c r="E31" s="2" t="s">
@@ -2968,7 +2969,7 @@
         <v>374</v>
       </c>
       <c r="D32" s="9">
-        <v>283107.94817825599</v>
+        <v>2.83107948178256E-9</v>
       </c>
       <c r="E32" s="5" t="s">
         <v>293</v>
@@ -3004,7 +3005,7 @@
       <c r="C33" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>0.181130959065747</v>
       </c>
       <c r="E33" s="2" t="s">
@@ -3041,7 +3042,7 @@
       <c r="C34" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>2.2851914650698E-2</v>
       </c>
       <c r="E34" s="2" t="s">
@@ -3078,7 +3079,7 @@
       <c r="C35" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>0.173990062260864</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -3115,7 +3116,7 @@
       <c r="C36" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>1.2793762003440999E-2</v>
       </c>
       <c r="E36" s="2" t="s">
@@ -3150,7 +3151,7 @@
         <v>374</v>
       </c>
       <c r="D37" s="9">
-        <v>4479283.9422576101</v>
+        <v>4.4792839422576103E-8</v>
       </c>
       <c r="E37" s="7" t="s">
         <v>316</v>
@@ -3188,7 +3189,7 @@
         <v>374</v>
       </c>
       <c r="D38" s="9">
-        <v>1400242.92143385</v>
+        <v>1.4002429214338501E-8</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>318</v>
@@ -3223,7 +3224,7 @@
       <c r="C39" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
         <v>2.08379530536593E-4</v>
       </c>
       <c r="E39" s="5" t="s">
@@ -3260,7 +3261,7 @@
       <c r="C40" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <v>0.16822198597351901</v>
       </c>
       <c r="E40" s="2" t="s">
@@ -3297,7 +3298,7 @@
       <c r="C41" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="1">
         <v>5.8266588140957597E-3</v>
       </c>
       <c r="E41" s="2" t="s">
@@ -3334,7 +3335,7 @@
       <c r="C42" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>0.86423118750254002</v>
       </c>
       <c r="E42" s="2" t="s">
@@ -3371,7 +3372,7 @@
       <c r="C43" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
         <v>0.226278892887955</v>
       </c>
       <c r="E43" s="2" t="s">
@@ -3408,7 +3409,7 @@
       <c r="C44" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="1">
         <v>0.38503720273485298</v>
       </c>
       <c r="E44" s="2" t="s">
@@ -3445,7 +3446,7 @@
       <c r="C45" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="1">
         <v>0.38966087811461497</v>
       </c>
       <c r="E45" s="2" t="s">
@@ -3481,7 +3482,7 @@
       <c r="C46" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="1">
         <v>3.80329431931829E-2</v>
       </c>
       <c r="E46" s="2" t="s">
@@ -3518,7 +3519,7 @@
       <c r="C47" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="1">
         <v>1.94909385586482E-2</v>
       </c>
       <c r="E47" s="2" t="s">
@@ -3555,7 +3556,7 @@
       <c r="C48" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="1">
         <v>6.3139109028043996E-3</v>
       </c>
       <c r="E48" s="2" t="s">
@@ -3592,7 +3593,7 @@
       <c r="C49" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="1">
         <v>4.5523817648905798E-2</v>
       </c>
       <c r="E49" s="2" t="s">
@@ -3629,7 +3630,7 @@
       <c r="C50" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="1">
         <v>0.18462451562339999</v>
       </c>
       <c r="E50" s="2" t="s">
@@ -3666,7 +3667,7 @@
       <c r="C51" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="1">
         <v>1.65969535353784E-4</v>
       </c>
       <c r="E51" s="2" t="s">
@@ -3703,7 +3704,7 @@
       <c r="C52" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="1">
         <v>0.13265546508012199</v>
       </c>
       <c r="E52" s="5" t="s">
@@ -3740,7 +3741,7 @@
       <c r="C53" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="1">
         <v>2.37839072927764E-2</v>
       </c>
       <c r="E53" s="2" t="s">
@@ -3777,7 +3778,7 @@
       <c r="C54" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="1">
         <v>1.33166306406753E-2</v>
       </c>
       <c r="E54" s="2" t="s">
@@ -3814,7 +3815,7 @@
       <c r="C55" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="1">
         <v>0.98970850600417803</v>
       </c>
       <c r="E55" s="2" t="s">
@@ -3851,7 +3852,7 @@
       <c r="C56" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="1">
         <v>3.83371655458229E-2</v>
       </c>
       <c r="E56" s="2" t="s">
@@ -3888,7 +3889,7 @@
       <c r="C57" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="1">
         <v>4.1902730229087401E-2</v>
       </c>
       <c r="E57" s="2" t="s">
@@ -3925,7 +3926,7 @@
       <c r="C58" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="1">
         <v>0.92087005115825904</v>
       </c>
       <c r="E58" s="2" t="s">
@@ -3962,7 +3963,7 @@
       <c r="C59" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="1">
         <v>2.9899389418534699E-3</v>
       </c>
       <c r="E59" s="2" t="s">
@@ -4000,7 +4001,7 @@
         <v>374</v>
       </c>
       <c r="D60" s="9">
-        <v>2.4960978010618099E-32</v>
+        <v>2.4960978010618101E-46</v>
       </c>
       <c r="E60" s="2" t="s">
         <v>320</v>
@@ -4035,7 +4036,7 @@
       <c r="C61" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="1">
         <v>0.57080594660208195</v>
       </c>
       <c r="E61" s="2" t="s">
@@ -4072,7 +4073,7 @@
       <c r="C62" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="1">
         <v>3.9833612146863699E-2</v>
       </c>
       <c r="E62" s="2" t="s">
@@ -4109,7 +4110,7 @@
       <c r="C63" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="1">
         <v>0.662305522339245</v>
       </c>
       <c r="E63" s="5" t="s">
@@ -4146,7 +4147,7 @@
       <c r="C64" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="1">
         <v>5.7077358439572803E-2</v>
       </c>
       <c r="E64" s="2" t="s">
@@ -4184,7 +4185,7 @@
         <v>374</v>
       </c>
       <c r="D65" s="9">
-        <v>7061776567.3121796</v>
+        <v>7.0617765673121794E-5</v>
       </c>
       <c r="E65" s="2" t="s">
         <v>219</v>
@@ -4220,7 +4221,7 @@
       <c r="C66" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="1">
         <v>3.5106362324375498E-3</v>
       </c>
       <c r="E66" s="2" t="s">
@@ -4257,7 +4258,7 @@
         <v>374</v>
       </c>
       <c r="D67" s="9">
-        <v>1.8736316802087899E-2</v>
+        <v>1.8736316802087901E-16</v>
       </c>
       <c r="E67" s="2" t="s">
         <v>302</v>
@@ -4292,7 +4293,7 @@
       <c r="C68" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="1">
         <v>0.28223929614052301</v>
       </c>
       <c r="E68" s="2" t="s">
@@ -4330,7 +4331,7 @@
         <v>374</v>
       </c>
       <c r="D69" s="9">
-        <v>1.5028993008290999E-3</v>
+        <v>1.5028993008291001E-16</v>
       </c>
       <c r="E69" s="2" t="s">
         <v>283</v>
@@ -4366,7 +4367,7 @@
       <c r="C70" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="1">
         <v>3.1243926127755301E-2</v>
       </c>
       <c r="E70" s="2" t="s">
@@ -4403,7 +4404,7 @@
       <c r="C71" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="1">
         <v>6.5715103410570103E-2</v>
       </c>
       <c r="E71" s="2" t="s">
@@ -4440,7 +4441,7 @@
       <c r="C72" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="1">
         <v>0.27251001536786701</v>
       </c>
       <c r="E72" s="2" t="s">
@@ -4478,7 +4479,7 @@
         <v>374</v>
       </c>
       <c r="D73" s="9">
-        <v>9.0649521283909191</v>
+        <v>9.0649521283909199E-14</v>
       </c>
       <c r="E73" s="7" t="s">
         <v>237</v>
@@ -4514,7 +4515,7 @@
       <c r="C74" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="1">
         <v>1.88189019904507E-2</v>
       </c>
       <c r="E74" s="2" t="s">
@@ -4551,7 +4552,7 @@
       <c r="C75" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="1">
         <v>3.7331317957546898E-4</v>
       </c>
       <c r="E75" s="2" t="s">
@@ -4588,7 +4589,7 @@
       <c r="C76" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D76">
+      <c r="D76" s="1">
         <v>6.1982659553184698E-3</v>
       </c>
       <c r="E76" s="2" t="s">
@@ -4625,7 +4626,7 @@
       <c r="C77" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="1">
         <v>0.192586393642037</v>
       </c>
       <c r="E77" s="2" t="s">
@@ -4662,7 +4663,7 @@
       <c r="C78" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="1">
         <v>0.70358077317367795</v>
       </c>
       <c r="E78" s="2" t="s">
@@ -4699,7 +4700,7 @@
       <c r="C79" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D79">
+      <c r="D79" s="1">
         <v>5.16966030823909E-2</v>
       </c>
       <c r="E79" s="5" t="s">
@@ -4736,7 +4737,7 @@
       <c r="C80" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="1">
         <v>0.25166982645240998</v>
       </c>
       <c r="E80" s="2" t="s">
@@ -4774,7 +4775,7 @@
         <v>374</v>
       </c>
       <c r="D81" s="9">
-        <v>348456.434947061</v>
+        <v>3.4845643494706101E-9</v>
       </c>
       <c r="E81" s="2" t="s">
         <v>195</v>
@@ -4810,7 +4811,7 @@
       <c r="C82" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D82">
+      <c r="D82" s="1">
         <v>1.5387522804187199E-3</v>
       </c>
       <c r="E82" s="5" t="s">
@@ -4847,7 +4848,7 @@
       <c r="C83" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D83">
+      <c r="D83" s="1">
         <v>7.1718969408590794E-2</v>
       </c>
       <c r="E83" s="2" t="s">
@@ -4884,7 +4885,7 @@
       <c r="C84" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="1">
         <v>0.31783276869523303</v>
       </c>
       <c r="E84" s="2" t="s">
@@ -4921,7 +4922,7 @@
       <c r="C85" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="1">
         <v>0.391625176271089</v>
       </c>
       <c r="E85" s="5" t="s">
@@ -4958,7 +4959,7 @@
       <c r="C86" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="1">
         <v>2.1506795848968901E-2</v>
       </c>
       <c r="E86" s="2" t="s">
@@ -4995,7 +4996,7 @@
       <c r="C87" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D87">
+      <c r="D87" s="1">
         <v>5.4944364903600003E-2</v>
       </c>
       <c r="E87" s="2" t="s">
@@ -5032,7 +5033,7 @@
       <c r="C88" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D88">
+      <c r="D88" s="1">
         <v>0.31349160347817701</v>
       </c>
       <c r="E88" s="2" t="s">
@@ -5069,7 +5070,7 @@
       <c r="C89" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D89">
+      <c r="D89" s="1">
         <v>0.69139626031457901</v>
       </c>
       <c r="E89" s="2" t="s">
@@ -5107,7 +5108,7 @@
         <v>374</v>
       </c>
       <c r="D90" s="9">
-        <v>677547813.44432795</v>
+        <v>6.7754781344432797E-6</v>
       </c>
       <c r="E90" s="2" t="s">
         <v>204</v>
@@ -5143,7 +5144,7 @@
       <c r="C91" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="1">
         <v>0.84586385485617499</v>
       </c>
       <c r="E91" s="2" t="s">
@@ -5179,7 +5180,7 @@
       <c r="C92" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="1">
         <v>0.208201272224386</v>
       </c>
       <c r="E92" s="2" t="s">
@@ -5216,7 +5217,7 @@
       <c r="C93" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="1">
         <v>2.22184537592575E-2</v>
       </c>
       <c r="E93" s="2" t="s">
@@ -5253,7 +5254,7 @@
       <c r="C94" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="1">
         <v>8.18347304238079E-2</v>
       </c>
       <c r="E94" s="2" t="s">
@@ -5290,7 +5291,7 @@
       <c r="C95" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="1">
         <v>8.8565403795990899E-2</v>
       </c>
       <c r="E95" s="2" t="s">
@@ -5327,7 +5328,7 @@
       <c r="C96" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="1">
         <v>2.4201512716478502E-3</v>
       </c>
       <c r="E96" s="2" t="s">
@@ -5363,7 +5364,7 @@
       <c r="C97" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="1">
         <v>0.396263008077958</v>
       </c>
       <c r="E97" s="2" t="s">
@@ -5401,7 +5402,7 @@
         <v>374</v>
       </c>
       <c r="D98" s="9">
-        <v>5411.5692360243302</v>
+        <v>5.41156923602433E-11</v>
       </c>
       <c r="E98" s="2" t="s">
         <v>313</v>
@@ -5438,7 +5439,7 @@
         <v>374</v>
       </c>
       <c r="D99" s="9">
-        <v>1.2423940249032101E-3</v>
+        <v>1.24239402490321E-17</v>
       </c>
       <c r="E99" s="2" t="s">
         <v>191</v>
@@ -5474,7 +5475,7 @@
       <c r="C100" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D100">
+      <c r="D100" s="1">
         <v>0.91870007832675504</v>
       </c>
       <c r="E100" s="2" t="s">
@@ -5510,7 +5511,7 @@
       <c r="C101" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D101">
+      <c r="D101" s="1">
         <v>0.75335862313205104</v>
       </c>
       <c r="E101" s="2" t="s">
@@ -5548,7 +5549,7 @@
         <v>374</v>
       </c>
       <c r="D102" s="9">
-        <v>2861347731.11063</v>
+        <v>2.8613477311106301E-5</v>
       </c>
       <c r="E102" s="2" t="s">
         <v>223</v>
@@ -5584,7 +5585,7 @@
       <c r="C103" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D103">
+      <c r="D103" s="1">
         <v>0.637345226549905</v>
       </c>
       <c r="E103" s="2" t="s">
@@ -5621,7 +5622,7 @@
       <c r="C104" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D104">
+      <c r="D104" s="1">
         <v>1.5053063958303601E-4</v>
       </c>
       <c r="E104" s="2" t="s">
@@ -5658,7 +5659,7 @@
       <c r="C105" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D105">
+      <c r="D105" s="1">
         <v>3.2012363330827598E-3</v>
       </c>
       <c r="E105" s="2" t="s">
@@ -5695,7 +5696,7 @@
       <c r="C106" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D106">
+      <c r="D106" s="1">
         <v>6.00306974755987E-2</v>
       </c>
       <c r="E106" s="2" t="s">
@@ -5732,7 +5733,7 @@
       <c r="C107" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D107">
+      <c r="D107" s="1">
         <v>1.59782465855246E-4</v>
       </c>
       <c r="E107" s="2" t="s">
@@ -5769,7 +5770,7 @@
       <c r="C108" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D108">
+      <c r="D108" s="1">
         <v>4.7213522599757699E-3</v>
       </c>
       <c r="E108" s="2" t="s">
@@ -5806,7 +5807,7 @@
       <c r="C109" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D109">
+      <c r="D109" s="1">
         <v>5.2163001866224103E-3</v>
       </c>
       <c r="E109" s="2" t="s">
@@ -5843,7 +5844,7 @@
       <c r="C110" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D110">
+      <c r="D110" s="1">
         <v>7.8574112591328399E-4</v>
       </c>
       <c r="E110" s="7" t="s">
@@ -5880,7 +5881,7 @@
       <c r="C111" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D111">
+      <c r="D111" s="1">
         <v>0.71939749259744701</v>
       </c>
       <c r="E111" s="2" t="s">
@@ -5917,7 +5918,7 @@
       <c r="C112" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D112">
+      <c r="D112" s="1">
         <v>0.40454188510301903</v>
       </c>
       <c r="E112" s="2" t="s">
@@ -5954,7 +5955,7 @@
       <c r="C113" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D113">
+      <c r="D113" s="1">
         <v>4.8732068003098502E-3</v>
       </c>
       <c r="E113" s="2" t="s">
@@ -5991,7 +5992,7 @@
       <c r="C114" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D114">
+      <c r="D114" s="1">
         <v>0.70875851050397098</v>
       </c>
       <c r="E114" s="5" t="s">
@@ -6028,7 +6029,7 @@
       <c r="C115" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D115">
+      <c r="D115" s="1">
         <v>0.134133250457484</v>
       </c>
       <c r="E115" s="2" t="s">
@@ -6065,7 +6066,7 @@
       <c r="C116" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D116">
+      <c r="D116" s="1">
         <v>4.42076652351742E-3</v>
       </c>
       <c r="E116" s="2" t="s">
@@ -6104,7 +6105,7 @@
       <c r="C117" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D117">
+      <c r="D117" s="1">
         <v>0.18238265490804001</v>
       </c>
       <c r="E117" s="2" t="s">
@@ -6141,7 +6142,7 @@
       <c r="C118" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D118">
+      <c r="D118" s="1">
         <v>0.197621757136558</v>
       </c>
       <c r="E118" s="2" t="s">
@@ -6178,7 +6179,7 @@
       <c r="C119" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D119">
+      <c r="D119" s="1">
         <v>0.24567145941011401</v>
       </c>
       <c r="E119" s="2" t="s">
@@ -6214,7 +6215,7 @@
       <c r="C120" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D120">
+      <c r="D120" s="1">
         <v>1</v>
       </c>
       <c r="E120" s="2" t="s">
@@ -6251,7 +6252,7 @@
       <c r="C121" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D121">
+      <c r="D121" s="1">
         <v>0.32036371526073198</v>
       </c>
       <c r="E121" s="2" t="s">
@@ -6288,7 +6289,7 @@
       <c r="C122" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D122">
+      <c r="D122" s="1">
         <v>4.5841403740706901E-2</v>
       </c>
       <c r="E122" s="2" t="s">
@@ -6325,7 +6326,7 @@
       <c r="C123" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D123">
+      <c r="D123" s="1">
         <v>5.7433119632003697E-2</v>
       </c>
       <c r="E123" s="5" t="s">
@@ -6362,7 +6363,7 @@
       <c r="C124" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D124">
+      <c r="D124" s="1">
         <v>1.15820777339506E-2</v>
       </c>
       <c r="E124" s="2" t="s">
@@ -6399,7 +6400,7 @@
       <c r="C125" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D125">
+      <c r="D125" s="1">
         <v>1.09477393273953E-3</v>
       </c>
       <c r="E125" s="2" t="s">
@@ -6437,7 +6438,7 @@
         <v>374</v>
       </c>
       <c r="D126" s="9">
-        <v>4.2432633411032601</v>
+        <v>4.2957949366351003E-14</v>
       </c>
       <c r="E126" s="2" t="s">
         <v>193</v>
@@ -6472,7 +6473,7 @@
       <c r="C127" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D127">
+      <c r="D127" s="1">
         <v>8.3565868816029204E-2</v>
       </c>
       <c r="E127" s="2" t="s">
@@ -6509,7 +6510,7 @@
       <c r="C128" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D128">
+      <c r="D128" s="1">
         <v>0.61707507745197399</v>
       </c>
       <c r="E128" s="2" t="s">
@@ -6547,7 +6548,7 @@
         <v>374</v>
       </c>
       <c r="D129" s="9">
-        <v>35029372.234125398</v>
+        <v>3.5029372234125401E-7</v>
       </c>
       <c r="E129" s="2" t="s">
         <v>192</v>
@@ -6583,7 +6584,7 @@
       <c r="C130" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D130">
+      <c r="D130" s="1">
         <v>2.0789532182140899E-2</v>
       </c>
       <c r="E130" s="2" t="s">
@@ -6620,7 +6621,7 @@
       <c r="C131" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D131">
+      <c r="D131" s="1">
         <v>0.31944709727239301</v>
       </c>
       <c r="E131" s="2" t="s">
@@ -6658,7 +6659,7 @@
         <v>374</v>
       </c>
       <c r="D132" s="9">
-        <v>5834314229.4191303</v>
+        <v>5.8343142294191302E-5</v>
       </c>
       <c r="E132" s="2" t="s">
         <v>247</v>
@@ -6694,7 +6695,7 @@
       <c r="C133" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D133">
+      <c r="D133" s="1">
         <v>1.6644959500271E-3</v>
       </c>
       <c r="E133" s="2" t="s">
@@ -6730,7 +6731,7 @@
       <c r="C134" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D134">
+      <c r="D134" s="1">
         <v>5.15063750136238E-3</v>
       </c>
       <c r="E134" s="2" t="s">
@@ -6767,7 +6768,7 @@
       <c r="C135" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D135">
+      <c r="D135" s="1">
         <v>2.41582363197352E-2</v>
       </c>
       <c r="E135" s="2" t="s">
@@ -6804,7 +6805,7 @@
       <c r="C136" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D136">
+      <c r="D136" s="1">
         <v>0.37714113978700903</v>
       </c>
       <c r="E136" s="2" t="s">
@@ -6840,7 +6841,7 @@
       <c r="C137" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D137">
+      <c r="D137" s="1">
         <v>0.33784332482653001</v>
       </c>
       <c r="E137" s="2" t="s">
@@ -6877,7 +6878,7 @@
       <c r="C138" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D138">
+      <c r="D138" s="1">
         <v>1.3699808042550801E-2</v>
       </c>
       <c r="E138" s="2" t="s">
@@ -6913,7 +6914,7 @@
       <c r="C139" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D139">
+      <c r="D139" s="1">
         <v>4.7006077888804197E-2</v>
       </c>
       <c r="E139" s="2" t="s">
@@ -6947,7 +6948,7 @@
       <c r="C140" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D140">
+      <c r="D140" s="1">
         <v>7.3414307165119196E-4</v>
       </c>
       <c r="E140" s="2" t="s">
@@ -6984,7 +6985,7 @@
       <c r="C141" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D141">
+      <c r="D141" s="1">
         <v>0.31844244245186398</v>
       </c>
       <c r="E141" s="2" t="s">
@@ -7022,7 +7023,7 @@
         <v>374</v>
       </c>
       <c r="D142" s="9">
-        <v>3.5055817350285103E-2</v>
+        <v>3.5055817350285102E-16</v>
       </c>
       <c r="E142" s="2" t="s">
         <v>206</v>
@@ -7057,7 +7058,7 @@
       <c r="C143" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D143">
+      <c r="D143" s="1">
         <v>0.71998174199157305</v>
       </c>
       <c r="E143" s="2" t="s">
@@ -7094,7 +7095,7 @@
       <c r="C144" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D144">
+      <c r="D144" s="1">
         <v>9.9098015421760902E-2</v>
       </c>
       <c r="E144" s="2" t="s">
@@ -7131,7 +7132,7 @@
       <c r="C145" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D145">
+      <c r="D145" s="1">
         <v>0.29712123338805202</v>
       </c>
       <c r="E145" s="2" t="s">
@@ -7168,7 +7169,7 @@
       <c r="C146" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D146">
+      <c r="D146" s="1">
         <v>5.29734824685483E-2</v>
       </c>
       <c r="E146" s="7" t="s">
@@ -7205,7 +7206,7 @@
       <c r="C147" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D147">
+      <c r="D147" s="1">
         <v>8.65018915713648E-3</v>
       </c>
       <c r="E147" s="2" t="s">
@@ -7242,7 +7243,7 @@
       <c r="C148" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D148">
+      <c r="D148" s="1">
         <v>0.119906553545096</v>
       </c>
       <c r="E148" s="2" t="s">
@@ -7279,7 +7280,7 @@
       <c r="C149" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D149">
+      <c r="D149" s="1">
         <v>5.3150984382344902E-3</v>
       </c>
       <c r="E149" s="2" t="s">
@@ -7316,7 +7317,7 @@
       <c r="C150" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D150">
+      <c r="D150" s="1">
         <v>2.2186350755732998E-3</v>
       </c>
       <c r="E150" s="2" t="s">
@@ -7353,7 +7354,7 @@
       <c r="C151" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D151">
+      <c r="D151" s="1">
         <v>4.7512184648556999E-2</v>
       </c>
       <c r="E151" s="2" t="s">
@@ -7390,7 +7391,7 @@
       <c r="C152" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D152">
+      <c r="D152" s="1">
         <v>0.15939040677403399</v>
       </c>
       <c r="E152" s="5" t="s">
@@ -7427,7 +7428,7 @@
       <c r="C153" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D153">
+      <c r="D153" s="1">
         <v>1.17861856665146E-2</v>
       </c>
       <c r="E153" s="2" t="s">
@@ -7463,7 +7464,7 @@
       <c r="C154" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D154">
+      <c r="D154" s="1">
         <v>6.0049986762664001E-2</v>
       </c>
       <c r="E154" s="2" t="s">
@@ -7500,7 +7501,7 @@
       <c r="C155" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D155">
+      <c r="D155" s="1">
         <v>0.62442197547863398</v>
       </c>
       <c r="E155" s="2" t="s">
@@ -7537,7 +7538,7 @@
       <c r="C156" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D156">
+      <c r="D156" s="1">
         <v>0.15939040677403399</v>
       </c>
       <c r="E156" s="2" t="s">
@@ -7574,7 +7575,7 @@
       <c r="C157" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D157">
+      <c r="D157" s="1">
         <v>0.300890687035128</v>
       </c>
       <c r="E157" s="2" t="s">
@@ -7611,7 +7612,7 @@
       <c r="C158" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D158">
+      <c r="D158" s="1">
         <v>6.5592949151269994E-2</v>
       </c>
       <c r="E158" s="2" t="s">
@@ -7648,7 +7649,7 @@
       <c r="C159" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D159">
+      <c r="D159" s="1">
         <v>8.4071223102123199E-2</v>
       </c>
       <c r="E159" s="2" t="s">
@@ -7685,7 +7686,7 @@
       <c r="C160" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D160">
+      <c r="D160" s="1">
         <v>2.9144332005850699E-3</v>
       </c>
       <c r="E160" s="2" t="s">
@@ -7721,7 +7722,7 @@
       <c r="C161" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D161">
+      <c r="D161" s="1">
         <v>4.9564235656245504E-4</v>
       </c>
       <c r="E161" s="5" t="s">
@@ -7758,7 +7759,7 @@
       <c r="C162" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D162">
+      <c r="D162" s="1">
         <v>7.8292294146410202E-2</v>
       </c>
       <c r="E162" s="2" t="s">
@@ -7795,7 +7796,7 @@
       <c r="C163" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D163">
+      <c r="D163" s="1">
         <v>2.5138066200090701E-3</v>
       </c>
       <c r="E163" s="2" t="s">
@@ -7832,7 +7833,7 @@
       <c r="C164" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D164">
+      <c r="D164" s="1">
         <v>0.39288318849133103</v>
       </c>
       <c r="E164" s="2" t="s">
@@ -7869,7 +7870,7 @@
       <c r="C165" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D165">
+      <c r="D165" s="1">
         <v>6.4910272297632604E-3</v>
       </c>
       <c r="E165" s="2" t="s">
@@ -7906,7 +7907,7 @@
       <c r="C166" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D166">
+      <c r="D166" s="1">
         <v>0.347684926165021</v>
       </c>
       <c r="E166" s="2" t="s">
@@ -7943,7 +7944,7 @@
       <c r="C167" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D167">
+      <c r="D167" s="1">
         <v>0.15237725580514599</v>
       </c>
       <c r="E167" s="2" t="s">
@@ -7979,7 +7980,7 @@
       <c r="C168" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D168">
+      <c r="D168" s="1">
         <v>6.4242947920458399E-2</v>
       </c>
       <c r="E168" s="2" t="s">
@@ -8016,7 +8017,7 @@
       <c r="C169" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D169">
+      <c r="D169" s="1">
         <v>0.101353833138701</v>
       </c>
       <c r="E169" s="2" t="s">
@@ -8053,7 +8054,7 @@
       <c r="C170" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D170">
+      <c r="D170" s="1">
         <v>4.5750425598842799E-2</v>
       </c>
       <c r="E170" s="2" t="s">
@@ -8090,7 +8091,7 @@
       <c r="C171" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D171">
+      <c r="D171" s="1">
         <v>6.2114739723029999E-2</v>
       </c>
       <c r="E171" s="2" t="s">
@@ -8127,7 +8128,7 @@
       <c r="C172" s="8" t="s">
         <v>374</v>
       </c>
-      <c r="D172">
+      <c r="D172" s="1">
         <v>4.9792357186444203E-2</v>
       </c>
       <c r="E172" s="2" t="s">
@@ -8164,7 +8165,7 @@
       <c r="C173" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D173">
+      <c r="D173" s="1">
         <v>0.27425805849962898</v>
       </c>
       <c r="E173" s="2" t="s">
@@ -8201,7 +8202,7 @@
       <c r="C174" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D174">
+      <c r="D174" s="1">
         <v>0.15571556670935499</v>
       </c>
       <c r="E174" s="2" t="s">
@@ -8238,7 +8239,7 @@
       <c r="C175" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D175">
+      <c r="D175" s="1">
         <v>7.03931880663555E-2</v>
       </c>
       <c r="E175" s="2" t="s">
@@ -8271,7 +8272,7 @@
       <c r="C176" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="D176">
+      <c r="D176" s="1">
         <v>0.42697534651230401</v>
       </c>
       <c r="E176" s="5" t="s">
@@ -8308,7 +8309,7 @@
       <c r="C177" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D177">
+      <c r="D177" s="1">
         <v>0.12962410896392901</v>
       </c>
       <c r="E177" s="2" t="s">
@@ -8344,7 +8345,7 @@
       <c r="C178" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D178">
+      <c r="D178" s="1">
         <v>0.20737500307370399</v>
       </c>
       <c r="E178" s="2" t="s">
@@ -8381,7 +8382,7 @@
       <c r="C179" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D179">
+      <c r="D179" s="1">
         <v>0.46722595574551801</v>
       </c>
       <c r="E179" s="2" t="s">
@@ -8418,7 +8419,7 @@
       <c r="C180" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D180">
+      <c r="D180" s="1">
         <v>8.6449184601804906E-3</v>
       </c>
       <c r="E180" s="2" t="s">
@@ -8456,7 +8457,7 @@
         <v>374</v>
       </c>
       <c r="D181" s="9">
-        <v>7307.1898261853203</v>
+        <v>7.3071898261853196E-11</v>
       </c>
       <c r="E181" s="2" t="s">
         <v>317</v>

</xml_diff>